<commit_message>
added Sprint Review 2 Protocol
</commit_message>
<xml_diff>
--- a/Org/Semester 3/Sprint_2.xlsx
+++ b/Org/Semester 3/Sprint_2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14820" windowHeight="6456"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14820" windowHeight="6450"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
   <si>
     <t>Sprint Review Protocol</t>
   </si>
@@ -117,30 +117,30 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Summe</t>
+  </si>
+  <si>
+    <t>Labels dynamisch ein-/ausblenden: Als Nutzer möchte ich Labels je nach Bedarf ein- oder ausblenden können, damit ich zwischen einer klaren Modellansicht und einer beschrifteten Ansicht wechseln kann. Akzeptanzkriterien: Labels können per UI-Element oder Geste ein-/ausgeblendet werden. Labels passen sich dynamisch an die aktuelle Sichtweise (Zoom, Rotation) an. Das Umschalten erfolgt ohne merkliche Verzögerung.</t>
+  </si>
+  <si>
+    <t>Quiz Ablauf designen (keine Implementierung): Als Entwickler möchte ich den Quizablauf klar definieren (Start, Fragen, Feedback, Ergebnis), damit die Implementierung konsistent und erweiterbar ist.</t>
+  </si>
+  <si>
+    <t>Labels mit erweiterten Informationen ausstatten: Als Nutzer möchte ich bei Bedarf zusätzliche Informationen über eine Herzkomponente abrufen können, damit ich mein Wissen vertiefen kann, ohne das Modell zu überladen. Akzeptanzkriterien: Erweiterte Informationen sind per Interaktion (z.B. Klick, Hover, Auswahl) abrufbar. Basisinformationen (Name der Komponente) bleiben weiterhin sichtbar.</t>
   </si>
   <si>
     <t>User Story:
 Als Nutzer möchte ich Labels klar und lesbar im VR-Interface angezeigt bekommen, damit ich die Herzkomponenten leicht identifizieren kann.
 Akzeptanzkriterien:
-Labels sind gut sichtbar und heben sich vom Hintergrund ab.
-Labels sind in VR aus verschiedenen Perspektiven lesbar.
-Das UI-Design entspricht dem einheitlichen Look &amp; Feel der Anwendung.
-Labels beeinträchtigen nicht die Sicht auf das Herzmodell.</t>
-  </si>
-  <si>
-    <t>Summe</t>
-  </si>
-  <si>
-    <t>Die Grundfunktion wurde in Sprint 1 implementiert, es kommt allerdings teilweise zu Darstellungsproblemen im Laufzeitmodus. In diesem Sprint wird an einer Optimierung gearbeitet.</t>
-  </si>
-  <si>
-    <t>Labels dynamisch ein-/ausblenden: Als Nutzer möchte ich Labels je nach Bedarf ein- oder ausblenden können, damit ich zwischen einer klaren Modellansicht und einer beschrifteten Ansicht wechseln kann. Akzeptanzkriterien: Labels können per UI-Element oder Geste ein-/ausgeblendet werden. Labels passen sich dynamisch an die aktuelle Sichtweise (Zoom, Rotation) an. Das Umschalten erfolgt ohne merkliche Verzögerung.</t>
-  </si>
-  <si>
-    <t>Labels mit erweiterten Informationen ausstatten: Als Nutzer möchte ich bei Bedarf zusätzliche Informationen über eine Herzkomponente abrufen können, damit ich mein Wissen vertiefen kann, ohne das Modell zu überladen. Akzeptanzkriterien: Erweiterte Informationen sind per Interaktion (z.B. Klick, Hover, Auswahl) abrufbar. Basisinformationen (Name der Komponente) bleiben weiterhin sichtbar. Erweiterte Inhalte sind fachlich korrekt und didaktisch sinnvoll strukturiert.</t>
-  </si>
-  <si>
-    <t>Quiz Ablauf designen (keine Implementierung): Als Entwickler möchte ich den Quizablauf klar definieren (Start, Fragen, Feedback, Ergebnis), damit die Implementierung konsistent und erweiterbar ist.</t>
+Labels beeinträchtigen nicht die Sicht auf das Herzmodell. Jedes Herzsegment der Scene wird durch ein Label gekennzeichnet.</t>
+  </si>
+  <si>
+    <t>Die Grundfunktion wurde in Sprint 1 implementiert, es kommt allerdings teilweise zu Darstellungsproblemen im Laufzeitmodus. In diesem Sprint wurde an einer Optimierung gearbeitet. Durch anhaltende Probleme bei der Darstellung wurde eine alternative Lösung entwickelt, bei der Segmente durch Button- Klicks blinken.</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -428,7 +428,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -463,9 +463,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -862,47 +859,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="81" zoomScaleNormal="94" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" style="2" customWidth="1"/>
-    <col min="2" max="2" width="65.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.44140625" style="2"/>
-    <col min="8" max="8" width="34.5546875" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="11.44140625" style="2"/>
+    <col min="2" max="2" width="65.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.42578125" style="2"/>
+    <col min="8" max="8" width="34.5703125" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-    </row>
-    <row r="3" spans="1:9" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+    </row>
+    <row r="3" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -913,136 +910,136 @@
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="30" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="32">
+      <c r="B4" s="30"/>
+      <c r="C4" s="31">
         <v>2</v>
       </c>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="33"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="20" t="s">
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="32"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="34">
-        <v>45965.8125</v>
-      </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="36"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="20" t="s">
+      <c r="B5" s="20"/>
+      <c r="C5" s="33">
+        <v>45965.913194444445</v>
+      </c>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="35"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="35">
+      <c r="B6" s="20"/>
+      <c r="C6" s="34">
         <v>16</v>
       </c>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="36"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="20" t="s">
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="35"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="37" t="s">
+      <c r="B7" s="20"/>
+      <c r="C7" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="38"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="20" t="s">
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="37"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="28" t="s">
+      <c r="B8" s="20"/>
+      <c r="C8" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="29"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="20" t="s">
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="28"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="28" t="s">
+      <c r="B9" s="20"/>
+      <c r="C9" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="29"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="20" t="s">
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="28"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="28" t="s">
+      <c r="B10" s="20"/>
+      <c r="C10" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="29"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="20" t="s">
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="28"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="25" t="s">
+      <c r="B11" s="20"/>
+      <c r="C11" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="26"/>
-    </row>
-    <row r="12" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="22" t="s">
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="25"/>
+    </row>
+    <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="23"/>
-      <c r="C12" s="18" t="s">
+      <c r="B12" s="22"/>
+      <c r="C12" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="19"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="24" t="s">
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="18"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="24"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B14" s="23"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
@@ -1068,76 +1065,92 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="171.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>1</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C16" s="10">
         <v>6</v>
       </c>
-      <c r="D16" s="10"/>
+      <c r="D16" s="10">
+        <v>12</v>
+      </c>
       <c r="E16" s="11"/>
-      <c r="F16" s="7"/>
+      <c r="F16" s="7" t="s">
+        <v>33</v>
+      </c>
       <c r="G16" s="8"/>
       <c r="H16" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="109.2" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>2</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C17" s="14">
         <v>23</v>
       </c>
-      <c r="D17" s="10"/>
+      <c r="D17" s="10">
+        <v>24</v>
+      </c>
       <c r="E17" s="11"/>
-      <c r="F17" s="7"/>
+      <c r="F17" s="7" t="s">
+        <v>33</v>
+      </c>
       <c r="G17" s="8"/>
       <c r="H17" s="13"/>
     </row>
-    <row r="18" spans="1:8" ht="124.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>3</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C18" s="10">
         <v>35</v>
       </c>
-      <c r="D18" s="10"/>
+      <c r="D18" s="10">
+        <v>27</v>
+      </c>
       <c r="E18" s="11"/>
-      <c r="F18" s="7"/>
+      <c r="F18" s="7" t="s">
+        <v>33</v>
+      </c>
       <c r="G18" s="8"/>
       <c r="H18" s="9"/>
     </row>
-    <row r="19" spans="1:8" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A19" s="15">
+    <row r="19" spans="1:8" ht="63" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
         <v>4</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C19" s="9">
         <v>7</v>
       </c>
-      <c r="D19" s="10"/>
+      <c r="D19" s="10">
+        <v>6</v>
+      </c>
       <c r="E19" s="11"/>
-      <c r="F19" s="7"/>
+      <c r="F19" s="7" t="s">
+        <v>33</v>
+      </c>
       <c r="G19" s="8"/>
-      <c r="H19" s="16"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H19" s="15"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
-      <c r="B20" s="17" t="s">
-        <v>28</v>
+      <c r="B20" s="16" t="s">
+        <v>27</v>
       </c>
       <c r="C20" s="2">
         <f>SUM(C16:C19)</f>
@@ -1145,7 +1158,7 @@
       </c>
       <c r="D20" s="2">
         <f>SUM(D15:D19)</f>
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="E20" s="4">
         <f>SUM(E16:E19)</f>
@@ -1159,13 +1172,13 @@
       </c>
       <c r="H20" s="4"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
         <v>20</v>
       </c>
@@ -1193,7 +1206,7 @@
     <mergeCell ref="A14:H14"/>
     <mergeCell ref="C11:G11"/>
   </mergeCells>
-  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="70" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>